<commit_message>
Upload file changed logic
</commit_message>
<xml_diff>
--- a/seleniumTests/reportsData/TestData.xlsx
+++ b/seleniumTests/reportsData/TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACM3\acm-selenium\com.armedia.arkcase.uitests\src\com\armedia\arkcase\uitests\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja.paskova\.arkcase\seleniumTests\reportsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21405" windowHeight="2175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21405" windowHeight="2175"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Audit" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="32">
   <si>
     <t xml:space="preserve">Test Case Name </t>
   </si>
@@ -45,9 +45,6 @@
     <t>Results</t>
   </si>
   <si>
-    <t>MATTER SUMMARY</t>
-  </si>
-  <si>
     <t>Draft</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>generateAuditReportforFiles</t>
+  </si>
+  <si>
+    <t>CASE SUMMARY</t>
   </si>
 </sst>
 </file>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,102 +520,102 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -647,10 +647,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -664,87 +664,87 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>